<commit_message>
Update advisor metrics spreadsheet
</commit_message>
<xml_diff>
--- a/Heart Metric Dashboard (3).xlsx
+++ b/Heart Metric Dashboard (3).xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brand\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://empoweredadvisor-my.sharepoint.com/personal/brandon_empoweryouradvisor_com/Documents/HEART Dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFAA617C-64A3-4C39-A59A-59D40EA30915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{C4F71938-9075-40F3-ADA7-27D68E8A1B91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0BC8D077-B457-4C7F-9E3A-6EEC63E4FF0A}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5242,8 +5242,8 @@
   <dimension ref="A1:AH304"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6467,7 +6467,7 @@
         <v>33</v>
       </c>
       <c r="I22" s="9">
-        <v>529.11</v>
+        <v>74</v>
       </c>
       <c r="J22" s="8">
         <v>55</v>
@@ -6638,7 +6638,7 @@
       </c>
       <c r="I25" s="12">
         <f t="shared" si="4"/>
-        <v>0.5449717450057644</v>
+        <v>3.8966216216216218</v>
       </c>
       <c r="J25" s="12">
         <f t="shared" si="4"/>
@@ -6705,7 +6705,7 @@
       </c>
       <c r="I26" s="12">
         <f t="shared" si="5"/>
-        <v>0.41418608606905938</v>
+        <v>2.9614864864864865</v>
       </c>
       <c r="J26" s="12">
         <f t="shared" si="5"/>
@@ -16379,7 +16379,7 @@
         <v>63</v>
       </c>
       <c r="I190" s="9">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="J190" s="8">
         <v>53</v>
@@ -16556,7 +16556,7 @@
       </c>
       <c r="I193" s="12">
         <f t="shared" si="46"/>
-        <v>60.116666666666667</v>
+        <v>5.4651515151515149</v>
       </c>
       <c r="J193" s="12">
         <f t="shared" si="46"/>
@@ -16623,7 +16623,7 @@
       </c>
       <c r="I194" s="12">
         <f t="shared" si="47"/>
-        <v>30.741666666666664</v>
+        <v>2.7946969696969695</v>
       </c>
       <c r="J194" s="12">
         <f t="shared" si="47"/>

</xml_diff>